<commit_message>
12.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/October/Others/Price list 28-10-2020.xlsx
+++ b/2020/October/Others/Price list 28-10-2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -285,7 +285,10 @@
     <t>BL96</t>
   </si>
   <si>
-    <t>Murad = 01740883469</t>
+    <t>T130</t>
+  </si>
+  <si>
+    <t>Last Update: 10.11.2020</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -657,7 +660,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -863,7 +866,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1964,7 +1967,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2411,7 +2414,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2471,7 +2474,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2488,7 +2491,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2551,7 +2554,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2568,7 +2571,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2628,7 +2631,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2661,7 +2664,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2673,7 +2676,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2951,7 +2954,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2962,7 +2965,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3025,7 +3028,7 @@
       <c r="D4" s="30"/>
       <c r="E4" s="11"/>
       <c r="F4" s="31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
@@ -3168,10 +3171,10 @@
         <v>26</v>
       </c>
       <c r="G10" s="7">
-        <v>1160</v>
+        <v>1180</v>
       </c>
       <c r="H10" s="7">
-        <v>1250</v>
+        <v>1270</v>
       </c>
       <c r="I10" s="5"/>
     </row>
@@ -3357,13 +3360,13 @@
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="G18" s="7">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="H18" s="7">
-        <v>1490</v>
+        <v>1350</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -3380,13 +3383,13 @@
       <c r="D19" s="17"/>
       <c r="E19" s="6"/>
       <c r="F19" s="8" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="G19" s="7">
-        <v>1220</v>
+        <v>1370</v>
       </c>
       <c r="H19" s="7">
-        <v>1320</v>
+        <v>1490</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -3403,13 +3406,13 @@
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="8" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="G20" s="7">
-        <v>3610</v>
+        <v>1220</v>
       </c>
       <c r="H20" s="7">
-        <v>3890</v>
+        <v>1320</v>
       </c>
       <c r="I20" s="5"/>
       <c r="L20" s="8"/>
@@ -3427,13 +3430,13 @@
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="7">
+        <v>3610</v>
+      </c>
+      <c r="H21" s="7">
         <v>3890</v>
-      </c>
-      <c r="H21" s="7">
-        <v>4190</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -3450,13 +3453,13 @@
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G22" s="7">
-        <v>4280</v>
+        <v>3890</v>
       </c>
       <c r="H22" s="7">
-        <v>4590</v>
+        <v>4190</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -3473,13 +3476,13 @@
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G23" s="7">
-        <v>4180</v>
+        <v>4280</v>
       </c>
       <c r="H23" s="7">
-        <v>4490</v>
+        <v>4590</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -3496,13 +3499,13 @@
       <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="G24" s="7">
-        <v>5390</v>
+        <v>4180</v>
       </c>
       <c r="H24" s="7">
-        <v>5790</v>
+        <v>4490</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -3519,13 +3522,13 @@
       <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G25" s="7">
-        <v>3560</v>
+        <v>5390</v>
       </c>
       <c r="H25" s="7">
-        <v>3840</v>
+        <v>5790</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -3542,13 +3545,13 @@
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G26" s="7">
-        <v>3340</v>
+        <v>3560</v>
       </c>
       <c r="H26" s="7">
-        <v>3590</v>
+        <v>3840</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -3565,13 +3568,13 @@
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="8" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="G27" s="7">
-        <v>4500</v>
+        <v>3340</v>
       </c>
       <c r="H27" s="7">
-        <v>4790</v>
+        <v>3590</v>
       </c>
       <c r="I27" s="5"/>
     </row>
@@ -3588,13 +3591,13 @@
       <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G28" s="7">
-        <v>3620</v>
+        <v>4500</v>
       </c>
       <c r="H28" s="7">
-        <v>3890</v>
+        <v>4790</v>
       </c>
       <c r="I28" s="5"/>
     </row>
@@ -3611,13 +3614,13 @@
       <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="7">
-        <v>4080</v>
+        <v>3620</v>
       </c>
       <c r="H29" s="7">
-        <v>4390</v>
+        <v>3890</v>
       </c>
       <c r="I29" s="5"/>
     </row>
@@ -3634,13 +3637,13 @@
       <c r="D30" s="5"/>
       <c r="E30" s="6"/>
       <c r="F30" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G30" s="7">
-        <v>4220</v>
+        <v>4080</v>
       </c>
       <c r="H30" s="7">
-        <v>4540</v>
+        <v>4390</v>
       </c>
       <c r="I30" s="5"/>
     </row>
@@ -3659,13 +3662,13 @@
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G31" s="7">
-        <v>3640</v>
+        <v>4220</v>
       </c>
       <c r="H31" s="7">
-        <v>3890</v>
+        <v>4540</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -3684,13 +3687,13 @@
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G32" s="7">
-        <v>3710</v>
+        <v>3640</v>
       </c>
       <c r="H32" s="7">
-        <v>3990</v>
+        <v>3890</v>
       </c>
       <c r="I32" s="5"/>
     </row>
@@ -3707,17 +3710,15 @@
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
       <c r="F33" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G33" s="7">
-        <v>7350</v>
+        <v>3710</v>
       </c>
       <c r="H33" s="7">
-        <v>7990</v>
-      </c>
-      <c r="I33" s="5">
-        <v>700</v>
-      </c>
+        <v>3990</v>
+      </c>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
@@ -3732,16 +3733,16 @@
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G34" s="7">
-        <v>7890</v>
+        <v>7350</v>
       </c>
       <c r="H34" s="7">
-        <v>8490</v>
+        <v>7990</v>
       </c>
       <c r="I34" s="5">
-        <v>300</v>
+        <v>700</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="20.100000000000001" customHeight="1">
@@ -3757,15 +3758,17 @@
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G35" s="7">
-        <v>7790</v>
+        <v>7890</v>
       </c>
       <c r="H35" s="7">
-        <v>8290</v>
-      </c>
-      <c r="I35" s="5"/>
+        <v>8490</v>
+      </c>
+      <c r="I35" s="5">
+        <v>300</v>
+      </c>
     </row>
     <row r="36" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="8" t="s">
@@ -3780,13 +3783,13 @@
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G36" s="7">
-        <v>8310</v>
+        <v>7790</v>
       </c>
       <c r="H36" s="7">
-        <v>8990</v>
+        <v>8290</v>
       </c>
       <c r="I36" s="5"/>
     </row>
@@ -3802,16 +3805,16 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="6"/>
-      <c r="F37" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G37" s="18">
-        <v>7800</v>
-      </c>
-      <c r="H37" s="18">
-        <v>8390</v>
-      </c>
-      <c r="I37" s="17"/>
+      <c r="F37" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" s="7">
+        <v>8310</v>
+      </c>
+      <c r="H37" s="7">
+        <v>8990</v>
+      </c>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="8" t="s">
@@ -3825,16 +3828,16 @@
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G38" s="7">
-        <v>8450</v>
-      </c>
-      <c r="H38" s="7">
-        <v>8990</v>
-      </c>
-      <c r="I38" s="5"/>
+      <c r="F38" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="18">
+        <v>7800</v>
+      </c>
+      <c r="H38" s="18">
+        <v>8390</v>
+      </c>
+      <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
@@ -3849,13 +3852,13 @@
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="8" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="G39" s="7">
-        <v>9300</v>
+        <v>8450</v>
       </c>
       <c r="H39" s="7">
-        <v>9790</v>
+        <v>8990</v>
       </c>
       <c r="I39" s="5"/>
     </row>
@@ -3874,13 +3877,13 @@
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G40" s="7">
-        <v>10340</v>
+        <v>9300</v>
       </c>
       <c r="H40" s="7">
-        <v>10990</v>
+        <v>9790</v>
       </c>
       <c r="I40" s="5"/>
     </row>
@@ -3896,9 +3899,15 @@
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
+      <c r="F41" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="7">
+        <v>10340</v>
+      </c>
+      <c r="H41" s="7">
+        <v>10990</v>
+      </c>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1">

</xml_diff>